<commit_message>
Add Robo Dog UML diagrams and update Excel
</commit_message>
<xml_diff>
--- a/試験準備/試験準備/ユースケース駆動開発_分析設計書_試験用テンプレート.xlsx
+++ b/試験準備/試験準備/ユースケース駆動開発_分析設計書_試験用テンプレート.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryo01/Desktop/develop/ohara_uml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k_nishida\Desktop\develop\ohara_uml\試験準備\試験準備\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEDD269-EB70-0749-96AE-0BC246902CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646F188B-4B0D-4220-B9D7-51C63A1B0C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="企画書" sheetId="14" r:id="rId1"/>
@@ -285,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1137,27 +1137,156 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="56" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1166,135 +1295,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="56" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1646,6 +1646,55 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>241935</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0B5E20-745C-4689-857E-D3F1A01E8805}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="469900"/>
+          <a:ext cx="8992235" cy="3733800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1988,13 +2037,13 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2038,7 +2087,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:D2"/>
@@ -2067,9 +2116,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="122" t="s">
         <v>24</v>
       </c>
@@ -2096,43 +2145,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="125"/>
       <c r="B2" s="126"/>
       <c r="C2" s="126"/>
       <c r="D2" s="127"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="65"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="63"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="125"/>
       <c r="B3" s="126"/>
       <c r="C3" s="126"/>
       <c r="D3" s="127"/>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="66"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" thickBot="1">
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="64"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="128"/>
       <c r="B4" s="129"/>
       <c r="C4" s="129"/>
@@ -2142,14 +2191,14 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="67"/>
-    </row>
-    <row r="5" spans="1:15" ht="19" thickTop="1"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="65"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="O2:O4"/>
@@ -2181,9 +2230,9 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -2210,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2227,8 +2276,8 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
-    <row r="4" spans="1:15" ht="27">
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="4" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2242,7 +2291,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="27">
+    <row r="5" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2256,7 +2305,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="27">
+    <row r="6" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2270,7 +2319,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="27">
+    <row r="7" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2284,7 +2333,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="27">
+    <row r="8" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2298,7 +2347,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="27">
+    <row r="9" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -2312,7 +2361,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="27">
+    <row r="10" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2326,7 +2375,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:15" ht="27">
+    <row r="11" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2340,7 +2389,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="27">
+    <row r="12" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2354,7 +2403,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="27">
+    <row r="13" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2368,7 +2417,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="27">
+    <row r="14" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2382,7 +2431,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:15" ht="27">
+    <row r="15" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2396,7 +2445,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:15" ht="27">
+    <row r="16" spans="1:15" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2410,7 +2459,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="2:13" ht="27">
+    <row r="17" spans="2:13" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2424,7 +2473,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="2:13" ht="27">
+    <row r="18" spans="2:13" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2438,7 +2487,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="2:13" ht="27">
+    <row r="19" spans="2:13" ht="26.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2480,9 +2529,9 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="26" t="s">
         <v>6</v>
       </c>
@@ -2509,7 +2558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2526,7 +2575,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:D2"/>
@@ -2551,13 +2600,13 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
@@ -2584,7 +2633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="35"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -2601,7 +2650,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:D2"/>
@@ -2615,6 +2664,7 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2629,9 +2679,9 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="39" t="s">
         <v>8</v>
       </c>
@@ -2658,7 +2708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="42"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -2675,7 +2725,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="M1:N1"/>
@@ -2703,15 +2753,15 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68"/>
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2732,237 +2782,230 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
-      <c r="A2" s="71"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="65"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="85" t="s">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="63"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="66"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" thickBot="1">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="76"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="64"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="67"/>
-    </row>
-    <row r="5" spans="1:15" ht="20" thickTop="1" thickBot="1"/>
-    <row r="6" spans="1:15" ht="22" thickTop="1" thickBot="1">
-      <c r="B6" s="80" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="65"/>
+    </row>
+    <row r="5" spans="1:15" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="6" spans="1:15" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="84"/>
-    </row>
-    <row r="7" spans="1:15" ht="22" thickTop="1" thickBot="1">
-      <c r="B7" s="63" t="s">
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="49"/>
+    </row>
+    <row r="7" spans="1:15" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="59"/>
-    </row>
-    <row r="8" spans="1:15" ht="21" thickBot="1">
-      <c r="B8" s="45" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="84"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62"/>
-    </row>
-    <row r="9" spans="1:15" ht="21" thickBot="1">
-      <c r="B9" s="45" t="s">
+      <c r="C8" s="81"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87"/>
+    </row>
+    <row r="9" spans="1:15" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="62"/>
-    </row>
-    <row r="10" spans="1:15" ht="58.5" customHeight="1" thickBot="1">
-      <c r="B10" s="45" t="s">
+      <c r="C9" s="81"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="87"/>
+    </row>
+    <row r="10" spans="1:15" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="51"/>
-    </row>
-    <row r="11" spans="1:15" ht="21" thickBot="1">
-      <c r="B11" s="45" t="s">
+      <c r="C10" s="81"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="90"/>
+    </row>
+    <row r="11" spans="1:15" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="62"/>
-    </row>
-    <row r="12" spans="1:15" ht="21" thickBot="1">
-      <c r="B12" s="45" t="s">
+      <c r="C11" s="81"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="87"/>
+    </row>
+    <row r="12" spans="1:15" ht="20.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="56"/>
-    </row>
-    <row r="13" spans="1:15" ht="219.75" customHeight="1" thickBot="1">
-      <c r="B13" s="45" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="80"/>
+    </row>
+    <row r="13" spans="1:15" ht="219.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="51"/>
-    </row>
-    <row r="14" spans="1:15" ht="75" customHeight="1" thickBot="1">
-      <c r="B14" s="45" t="s">
+      <c r="C13" s="81"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="90"/>
+    </row>
+    <row r="14" spans="1:15" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="51"/>
-    </row>
-    <row r="15" spans="1:15" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B15" s="47" t="s">
+      <c r="C14" s="81"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="90"/>
+    </row>
+    <row r="15" spans="1:15" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="54"/>
-    </row>
-    <row r="16" spans="1:15" ht="19" thickTop="1"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="97"/>
+    </row>
+    <row r="16" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:M6"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="J2:L4"/>
-    <mergeCell ref="M2:N4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:M13"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="D15:M15"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D7:M7"/>
@@ -2975,11 +3018,18 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D13:M13"/>
-    <mergeCell ref="D14:M14"/>
-    <mergeCell ref="D15:M15"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="J2:L4"/>
+    <mergeCell ref="M2:N4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2998,9 +3048,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="98" t="s">
         <v>21</v>
       </c>
@@ -3027,43 +3077,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="101"/>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
       <c r="D2" s="103"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="65"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="63"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="101"/>
       <c r="B3" s="102"/>
       <c r="C3" s="102"/>
       <c r="D3" s="103"/>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="66"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" thickBot="1">
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="64"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="104"/>
       <c r="B4" s="105"/>
       <c r="C4" s="105"/>
@@ -3073,30 +3123,30 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="67"/>
-    </row>
-    <row r="5" spans="1:15" ht="19" thickTop="1"/>
-    <row r="6" spans="1:15" ht="28" customHeight="1"/>
-    <row r="7" spans="1:15" ht="28" customHeight="1"/>
-    <row r="8" spans="1:15" ht="28" customHeight="1"/>
-    <row r="9" spans="1:15" ht="28" customHeight="1"/>
-    <row r="10" spans="1:15" ht="28" customHeight="1"/>
-    <row r="11" spans="1:15" ht="28" customHeight="1"/>
-    <row r="12" spans="1:15" ht="28" customHeight="1"/>
-    <row r="13" spans="1:15" ht="28" customHeight="1"/>
-    <row r="14" spans="1:15" ht="28" customHeight="1"/>
-    <row r="15" spans="1:15" ht="28" customHeight="1"/>
-    <row r="16" spans="1:15" ht="28" customHeight="1"/>
-    <row r="17" ht="28" customHeight="1"/>
-    <row r="18" ht="28" customHeight="1"/>
-    <row r="19" ht="28" customHeight="1"/>
-    <row r="20" ht="28" customHeight="1"/>
-    <row r="21" ht="18" customHeight="1"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="65"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="6" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="8" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="9" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="12" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="19" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="O2:O4"/>
@@ -3127,9 +3177,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="107" t="s">
         <v>22</v>
       </c>
@@ -3156,43 +3206,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="110"/>
       <c r="B2" s="111"/>
       <c r="C2" s="111"/>
       <c r="D2" s="112"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="65"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="63"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="110"/>
       <c r="B3" s="111"/>
       <c r="C3" s="111"/>
       <c r="D3" s="112"/>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="66"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" thickBot="1">
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="64"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="113"/>
       <c r="B4" s="114"/>
       <c r="C4" s="114"/>
@@ -3202,30 +3252,30 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="67"/>
-    </row>
-    <row r="5" spans="1:15" ht="19" thickTop="1"/>
-    <row r="6" spans="1:15" ht="28" customHeight="1"/>
-    <row r="7" spans="1:15" ht="28" customHeight="1"/>
-    <row r="8" spans="1:15" ht="28" customHeight="1"/>
-    <row r="9" spans="1:15" ht="28" customHeight="1"/>
-    <row r="10" spans="1:15" ht="28" customHeight="1"/>
-    <row r="11" spans="1:15" ht="28" customHeight="1"/>
-    <row r="12" spans="1:15" ht="28" customHeight="1"/>
-    <row r="13" spans="1:15" ht="28" customHeight="1"/>
-    <row r="14" spans="1:15" ht="28" customHeight="1"/>
-    <row r="15" spans="1:15" ht="28" customHeight="1"/>
-    <row r="16" spans="1:15" ht="28" customHeight="1"/>
-    <row r="17" ht="28" customHeight="1"/>
-    <row r="18" ht="28" customHeight="1"/>
-    <row r="19" ht="28" customHeight="1"/>
-    <row r="20" ht="28" customHeight="1"/>
-    <row r="21" ht="18" customHeight="1"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="65"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="6" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="8" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="9" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="12" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="19" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="O2:O4"/>
@@ -3256,9 +3306,9 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" thickTop="1">
+    <row r="1" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="116" t="s">
         <v>23</v>
       </c>
@@ -3285,7 +3335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" thickBot="1">
+    <row r="2" spans="1:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="119"/>
       <c r="B2" s="120"/>
       <c r="C2" s="120"/>
@@ -3302,7 +3352,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="19" thickTop="1"/>
+    <row r="3" spans="1:15" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:D2"/>
@@ -3320,6 +3370,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="04574505-c322-4981-8ebb-5d25af8d4de8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101009C7952A5A25B2543AB99BC9B879A46ED" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="00b68e39924f37ea7b1a5acaf8857e0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8" xmlns:ns3="04574505-c322-4981-8ebb-5d25af8d4de8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1760b117eeeff4f4de69ce8d4b9089c6" ns2:_="" ns3:_="">
     <xsd:import namespace="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8"/>
@@ -3520,34 +3590,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="04574505-c322-4981-8ebb-5d25af8d4de8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A751DC5-F95E-46D4-AE54-08C8CEF11ED7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072AC1A6-4679-477C-AACD-93A3EE4A7F07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="04574505-c322-4981-8ebb-5d25af8d4de8"/>
+    <ds:schemaRef ds:uri="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C6F0FCF-3624-4DDB-A171-8F40C8BCB351}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C6F0FCF-3624-4DDB-A171-8F40C8BCB351}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072AC1A6-4679-477C-AACD-93A3EE4A7F07}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A751DC5-F95E-46D4-AE54-08C8CEF11ED7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="098a3c11-7ac2-46ba-89ce-8b2d5c9f76f8"/>
+    <ds:schemaRef ds:uri="04574505-c322-4981-8ebb-5d25af8d4de8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>